<commit_message>
almost got team spreadsheet working
</commit_message>
<xml_diff>
--- a/data/teams.xlsx
+++ b/data/teams.xlsx
@@ -20,21 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arkansas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Michigan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fri Jul  5 06:18:15 2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abbreviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shortDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nickname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standingSummary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri Jul  5 06:51:04 2024</t>
   </si>
 </sst>
 </file>
@@ -142,23 +157,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -342,16 +340,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,18 +358,31 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
+      <c r="I2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>